<commit_message>
UPDATED XPATHS IN CREATE LEAD
</commit_message>
<xml_diff>
--- a/src/main/resources/zoho_crm_leads.xlsx
+++ b/src/main/resources/zoho_crm_leads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JKS\Education\Personal\Online courses\Naresh\Java\IntelliJ workspaces\Pallet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B468A4-0E68-4165-B534-B67E02F0365B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FA69DA-5F02-4D0B-916F-2F81041F20A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{F02BB07E-4D36-4D23-A3C9-990753E6F2FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{F02BB07E-4D36-4D23-A3C9-990753E6F2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="website" sheetId="2" r:id="rId1"/>
@@ -77,78 +77,18 @@
     <t>//div[@class = 'left-menu-row2 leftmenu-modulelist dF flexDC teamspc-module-lists lyteScrollBar']</t>
   </si>
   <si>
-    <t>//input[@tabindex = 6]</t>
-  </si>
-  <si>
-    <t>//div[@tabindex  = 7]</t>
-  </si>
-  <si>
     <t>//lyte-drop-item[@data-value  = 'Mr.']</t>
   </si>
   <si>
-    <t>//input[@tabindex  = 7]</t>
-  </si>
-  <si>
-    <t>//input[@tabindex  = 8]</t>
-  </si>
-  <si>
-    <t>//input[@tabindex  = 9]</t>
-  </si>
-  <si>
-    <t>//input[@tabindex  = 10]</t>
-  </si>
-  <si>
-    <t>//input[@tabindex  = 11]</t>
-  </si>
-  <si>
-    <t>//input[@tabindex  = 13]</t>
-  </si>
-  <si>
-    <t>//input[@tabindex  = 14]</t>
-  </si>
-  <si>
-    <t>//div[@tabindex  = 15]</t>
-  </si>
-  <si>
     <t>//lyte-drop-item[@data-value  = 'Web Download']</t>
   </si>
   <si>
-    <t>//div[@tabIndex = 16]</t>
-  </si>
-  <si>
     <t>//lyte-drop-item[@data-value = 'Contacted']</t>
   </si>
   <si>
-    <t>//div[@tabIndex = 17]</t>
-  </si>
-  <si>
     <t>//lyte-drop-item[@data-value = 'Large Enterprise']</t>
   </si>
   <si>
-    <t>//input[@tabIndex = 19]</t>
-  </si>
-  <si>
-    <t>//input[@tabIndex = 22]</t>
-  </si>
-  <si>
-    <t>//input[@tabIndex = 24]</t>
-  </si>
-  <si>
-    <t>//input[@tabIndex = 25]</t>
-  </si>
-  <si>
-    <t>//input[@tabIndex = 26]</t>
-  </si>
-  <si>
-    <t>//input[@tabIndex = 27]</t>
-  </si>
-  <si>
-    <t>//input[@tabIndex = 28]</t>
-  </si>
-  <si>
-    <t>//input[@tabIndex = 29]</t>
-  </si>
-  <si>
     <t>//div[@role = 'button' and @aria-label = 'Leads']</t>
   </si>
   <si>
@@ -678,6 +618,66 @@
   </si>
   <si>
     <t>lead_source_inp</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby = 'Crm_Leads_COMPANY_label']</t>
+  </si>
+  <si>
+    <t>//div[@aria-label = 'Salutation']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_FIRSTNAME_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_LASTNAME_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_DESIGNATION_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_EMAIL_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_PHONE_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_MOBILE_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_WEBSITE_label']</t>
+  </si>
+  <si>
+    <t>//div[@aria-labelledby='Crm_Leads_LEADSOURCE_label']</t>
+  </si>
+  <si>
+    <t>//div[@aria-labelledby='Crm_Leads_STATUS_label']</t>
+  </si>
+  <si>
+    <t>//div[@aria-labelledby='Crm_Leads_INDUSTRY_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_ANNUALREVENUE_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_SKYPEIDENTITY_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_TWITTER_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_LANE_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_CITY_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_STATE_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_CODE_label']</t>
+  </si>
+  <si>
+    <t>//input[@aria-labelledby='Crm_Leads_COUNTRY_label']</t>
   </si>
 </sst>
 </file>
@@ -1053,13 +1053,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1070,117 +1070,117 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1191,29 +1191,29 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1226,345 +1226,345 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC8FF67-269C-46AD-9364-6F65B6266DBB}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.21875" customWidth="1"/>
     <col min="3" max="3" width="55" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>199</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>203</v>
       </c>
       <c r="C12" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>206</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>207</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>208</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>209</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>210</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>211</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>212</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>213</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>214</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>215</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE29B49F-3A39-40BE-8643-C05720C27E2F}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1590,156 +1590,156 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1752,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99338FFD-0177-4432-85FA-5216F6EBC65B}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1765,200 +1765,200 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="C14" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="C16" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C18" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1972,7 +1972,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1984,112 +1984,112 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2115,67 +2115,67 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>